<commit_message>
Added shablons with by Ksendzov check-list
</commit_message>
<xml_diff>
--- a/Check-list/Shablon_.xlsx
+++ b/Check-list/Shablon_.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="19020" windowHeight="9855" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="19020" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Check-list" sheetId="1" r:id="rId1"/>
@@ -1367,6 +1367,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1376,47 +1412,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2389,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -2408,41 +2408,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="98" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="105" t="s">
+      <c r="I1" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="109" t="s">
+      <c r="J1" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="106" t="s">
+      <c r="K1" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="109" t="s">
+      <c r="L1" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="106" t="s">
+      <c r="M1" s="97" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       <c r="L3" s="45"/>
       <c r="M3" s="35"/>
     </row>
-    <row r="4" spans="1:13" ht="30">
+    <row r="4" spans="1:13" ht="45">
       <c r="A4" s="45"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -2546,7 +2546,7 @@
       <c r="L6" s="45"/>
       <c r="M6" s="35"/>
     </row>
-    <row r="7" spans="1:13" ht="45">
+    <row r="7" spans="1:13" ht="60">
       <c r="A7" s="45"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -2769,7 +2769,7 @@
       <c r="L19" s="45"/>
       <c r="M19" s="35"/>
     </row>
-    <row r="20" spans="1:13" ht="60">
+    <row r="20" spans="1:13" ht="75">
       <c r="A20" s="41"/>
       <c r="B20" s="37"/>
       <c r="C20" s="37"/>
@@ -2894,7 +2894,7 @@
       <c r="L26" s="45"/>
       <c r="M26" s="35"/>
     </row>
-    <row r="27" spans="1:13" ht="30">
+    <row r="27" spans="1:13" ht="45">
       <c r="A27" s="45"/>
       <c r="B27" s="45"/>
       <c r="C27" s="45"/>
@@ -2936,7 +2936,7 @@
       <c r="L29" s="45"/>
       <c r="M29" s="35"/>
     </row>
-    <row r="30" spans="1:13" ht="30">
+    <row r="30" spans="1:13" ht="45">
       <c r="A30" s="45"/>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
@@ -3064,7 +3064,7 @@
       <c r="L38" s="45"/>
       <c r="M38" s="35"/>
     </row>
-    <row r="39" spans="1:13" ht="30">
+    <row r="39" spans="1:13" ht="45">
       <c r="A39" s="41"/>
       <c r="B39" s="41"/>
       <c r="C39" s="41"/>
@@ -3196,7 +3196,7 @@
       <c r="L45" s="45"/>
       <c r="M45" s="35"/>
     </row>
-    <row r="46" spans="1:13" ht="30">
+    <row r="46" spans="1:13" ht="45">
       <c r="A46" s="45"/>
       <c r="B46" s="35"/>
       <c r="C46" s="35"/>
@@ -3247,7 +3247,7 @@
       <c r="L48" s="45"/>
       <c r="M48" s="35"/>
     </row>
-    <row r="49" spans="1:13" ht="45">
+    <row r="49" spans="1:13" ht="60">
       <c r="A49" s="45"/>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
@@ -3419,7 +3419,7 @@
       <c r="L58" s="45"/>
       <c r="M58" s="35"/>
     </row>
-    <row r="59" spans="1:13" ht="75">
+    <row r="59" spans="1:13" ht="90">
       <c r="A59" s="41"/>
       <c r="B59" s="37"/>
       <c r="C59" s="37"/>
@@ -3483,7 +3483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -3503,48 +3503,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="76.5" customHeight="1">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="112" t="s">
+      <c r="F2" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="112" t="s">
+      <c r="G2" s="103" t="s">
         <v>170</v>
       </c>
-      <c r="H2" s="112" t="s">
+      <c r="H2" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="110" t="s">
+      <c r="I2" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="112" t="s">
+      <c r="J2" s="103" t="s">
         <v>165</v>
       </c>
-      <c r="K2" s="112" t="s">
+      <c r="K2" s="103" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.5">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="106" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="92" t="s">
@@ -3571,9 +3571,9 @@
       <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11" ht="30">
-      <c r="A4" s="100"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
       <c r="D4" s="88" t="s">
         <v>140</v>
       </c>
@@ -3586,9 +3586,9 @@
       <c r="K4" s="45"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="100"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
       <c r="D5" s="89"/>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
@@ -3599,9 +3599,9 @@
       <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
       <c r="D6" s="90" t="s">
         <v>95</v>
       </c>
@@ -3614,9 +3614,9 @@
       <c r="K6" s="45"/>
     </row>
     <row r="7" spans="1:11" ht="35.25" customHeight="1">
-      <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
       <c r="D7" s="88" t="s">
         <v>98</v>
       </c>
@@ -3825,13 +3825,13 @@
       <c r="K20" s="41"/>
     </row>
     <row r="21" spans="1:11" ht="25.5">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="102" t="s">
+      <c r="B21" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="C21" s="96"/>
+      <c r="C21" s="108"/>
       <c r="D21" s="22"/>
       <c r="E21" s="83" t="str">
         <f>'Свойства дефекта'!A2</f>
@@ -3854,9 +3854,9 @@
       <c r="K21" s="44"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="100"/>
-      <c r="B22" s="103"/>
-      <c r="C22" s="97"/>
+      <c r="A22" s="105"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="109"/>
       <c r="D22" s="27"/>
       <c r="E22" s="28"/>
       <c r="F22" s="27"/>
@@ -3867,9 +3867,9 @@
       <c r="K22" s="45"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="100"/>
-      <c r="B23" s="103"/>
-      <c r="C23" s="97"/>
+      <c r="A23" s="105"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="27"/>
       <c r="E23" s="28"/>
       <c r="F23" s="27"/>
@@ -3880,9 +3880,9 @@
       <c r="K23" s="45"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="100"/>
-      <c r="B24" s="103"/>
-      <c r="C24" s="97"/>
+      <c r="A24" s="105"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="109"/>
       <c r="D24" s="27"/>
       <c r="E24" s="28"/>
       <c r="F24" s="27"/>
@@ -3893,9 +3893,9 @@
       <c r="K24" s="45"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="100"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="97"/>
+      <c r="A25" s="105"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="109"/>
       <c r="D25" s="45"/>
       <c r="E25" s="28"/>
       <c r="F25" s="27"/>
@@ -4016,13 +4016,13 @@
       <c r="K33" s="41"/>
     </row>
     <row r="34" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A34" s="99" t="s">
+      <c r="A34" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="102" t="s">
+      <c r="B34" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="C34" s="96"/>
+      <c r="C34" s="108"/>
       <c r="D34" s="22"/>
       <c r="E34" s="83"/>
       <c r="F34" s="24"/>
@@ -4031,9 +4031,9 @@
       <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="100"/>
-      <c r="B35" s="103"/>
-      <c r="C35" s="97"/>
+      <c r="A35" s="105"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="109"/>
       <c r="D35" s="27"/>
       <c r="E35" s="28"/>
       <c r="F35" s="27"/>
@@ -4042,9 +4042,9 @@
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="100"/>
-      <c r="B36" s="103"/>
-      <c r="C36" s="97"/>
+      <c r="A36" s="105"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="27"/>
       <c r="E36" s="28"/>
       <c r="F36" s="27"/>
@@ -4053,9 +4053,9 @@
       <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="100"/>
-      <c r="B37" s="103"/>
-      <c r="C37" s="97"/>
+      <c r="A37" s="105"/>
+      <c r="B37" s="107"/>
+      <c r="C37" s="109"/>
       <c r="D37" s="27"/>
       <c r="E37" s="28"/>
       <c r="F37" s="27"/>
@@ -4064,9 +4064,9 @@
       <c r="I37" s="28"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="100"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="98"/>
+      <c r="A38" s="105"/>
+      <c r="B38" s="107"/>
+      <c r="C38" s="110"/>
       <c r="D38" s="41"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
@@ -4075,13 +4075,13 @@
       <c r="I38" s="33"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="99" t="s">
+      <c r="A39" s="104" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="102" t="s">
+      <c r="B39" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="C39" s="96"/>
+      <c r="C39" s="108"/>
       <c r="D39" s="22"/>
       <c r="E39" s="83"/>
       <c r="F39" s="24"/>
@@ -4090,9 +4090,9 @@
       <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="100"/>
-      <c r="B40" s="103"/>
-      <c r="C40" s="97"/>
+      <c r="A40" s="105"/>
+      <c r="B40" s="107"/>
+      <c r="C40" s="109"/>
       <c r="D40" s="27"/>
       <c r="E40" s="28"/>
       <c r="F40" s="27"/>
@@ -4101,9 +4101,9 @@
       <c r="I40" s="28"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="100"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="97"/>
+      <c r="A41" s="105"/>
+      <c r="B41" s="107"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="27"/>
       <c r="E41" s="28"/>
       <c r="F41" s="27"/>
@@ -4112,9 +4112,9 @@
       <c r="I41" s="28"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="100"/>
-      <c r="B42" s="103"/>
-      <c r="C42" s="97"/>
+      <c r="A42" s="105"/>
+      <c r="B42" s="107"/>
+      <c r="C42" s="109"/>
       <c r="D42" s="27"/>
       <c r="E42" s="28"/>
       <c r="F42" s="27"/>
@@ -4123,9 +4123,9 @@
       <c r="I42" s="28"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="100"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="98"/>
+      <c r="A43" s="105"/>
+      <c r="B43" s="107"/>
+      <c r="C43" s="110"/>
       <c r="D43" s="41"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
@@ -4134,13 +4134,13 @@
       <c r="I43" s="33"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="99" t="s">
+      <c r="A44" s="104" t="s">
         <v>148</v>
       </c>
-      <c r="B44" s="102" t="s">
+      <c r="B44" s="106" t="s">
         <v>149</v>
       </c>
-      <c r="C44" s="96"/>
+      <c r="C44" s="108"/>
       <c r="D44" s="22"/>
       <c r="E44" s="83"/>
       <c r="F44" s="24"/>
@@ -4149,9 +4149,9 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="100"/>
-      <c r="B45" s="103"/>
-      <c r="C45" s="97"/>
+      <c r="A45" s="105"/>
+      <c r="B45" s="107"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="27"/>
       <c r="E45" s="28"/>
       <c r="F45" s="27"/>
@@ -4160,9 +4160,9 @@
       <c r="I45" s="28"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="100"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="97"/>
+      <c r="A46" s="105"/>
+      <c r="B46" s="107"/>
+      <c r="C46" s="109"/>
       <c r="D46" s="27"/>
       <c r="E46" s="28"/>
       <c r="F46" s="27"/>
@@ -4171,9 +4171,9 @@
       <c r="I46" s="28"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="100"/>
-      <c r="B47" s="103"/>
-      <c r="C47" s="97"/>
+      <c r="A47" s="105"/>
+      <c r="B47" s="107"/>
+      <c r="C47" s="109"/>
       <c r="D47" s="27"/>
       <c r="E47" s="28"/>
       <c r="F47" s="27"/>
@@ -4182,9 +4182,9 @@
       <c r="I47" s="28"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="100"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="98"/>
+      <c r="A48" s="105"/>
+      <c r="B48" s="107"/>
+      <c r="C48" s="110"/>
       <c r="D48" s="41"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
@@ -4193,13 +4193,13 @@
       <c r="I48" s="33"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="99" t="s">
+      <c r="A49" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="B49" s="102" t="s">
+      <c r="B49" s="106" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="96"/>
+      <c r="C49" s="108"/>
       <c r="D49" s="22"/>
       <c r="E49" s="83"/>
       <c r="F49" s="24"/>
@@ -4208,9 +4208,9 @@
       <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="100"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="97"/>
+      <c r="A50" s="105"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="109"/>
       <c r="D50" s="27"/>
       <c r="E50" s="28"/>
       <c r="F50" s="27"/>
@@ -4219,9 +4219,9 @@
       <c r="I50" s="28"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="100"/>
-      <c r="B51" s="103"/>
-      <c r="C51" s="97"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="109"/>
       <c r="D51" s="27"/>
       <c r="E51" s="28"/>
       <c r="F51" s="27"/>
@@ -4230,9 +4230,9 @@
       <c r="I51" s="28"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="100"/>
-      <c r="B52" s="103"/>
-      <c r="C52" s="97"/>
+      <c r="A52" s="105"/>
+      <c r="B52" s="107"/>
+      <c r="C52" s="109"/>
       <c r="D52" s="27"/>
       <c r="E52" s="28"/>
       <c r="F52" s="27"/>
@@ -4241,9 +4241,9 @@
       <c r="I52" s="28"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="100"/>
-      <c r="B53" s="103"/>
-      <c r="C53" s="98"/>
+      <c r="A53" s="105"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="110"/>
       <c r="D53" s="41"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
@@ -4252,13 +4252,13 @@
       <c r="I53" s="33"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="99" t="s">
+      <c r="A54" s="104" t="s">
         <v>152</v>
       </c>
-      <c r="B54" s="102" t="s">
+      <c r="B54" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="C54" s="96"/>
+      <c r="C54" s="108"/>
       <c r="D54" s="22"/>
       <c r="E54" s="83"/>
       <c r="F54" s="24"/>
@@ -4267,9 +4267,9 @@
       <c r="I54" s="26"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="100"/>
-      <c r="B55" s="103"/>
-      <c r="C55" s="97"/>
+      <c r="A55" s="105"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="109"/>
       <c r="D55" s="27"/>
       <c r="E55" s="28"/>
       <c r="F55" s="27"/>
@@ -4278,9 +4278,9 @@
       <c r="I55" s="28"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="100"/>
-      <c r="B56" s="103"/>
-      <c r="C56" s="97"/>
+      <c r="A56" s="105"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="109"/>
       <c r="D56" s="27"/>
       <c r="E56" s="28"/>
       <c r="F56" s="27"/>
@@ -4289,9 +4289,9 @@
       <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="100"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="97"/>
+      <c r="A57" s="105"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="109"/>
       <c r="D57" s="27"/>
       <c r="E57" s="28"/>
       <c r="F57" s="27"/>
@@ -4300,9 +4300,9 @@
       <c r="I57" s="28"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="100"/>
-      <c r="B58" s="103"/>
-      <c r="C58" s="98"/>
+      <c r="A58" s="105"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="110"/>
       <c r="D58" s="41"/>
       <c r="E58" s="33"/>
       <c r="F58" s="32"/>
@@ -4311,13 +4311,13 @@
       <c r="I58" s="33"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="99" t="s">
+      <c r="A59" s="104" t="s">
         <v>154</v>
       </c>
-      <c r="B59" s="102" t="s">
+      <c r="B59" s="106" t="s">
         <v>153</v>
       </c>
-      <c r="C59" s="96"/>
+      <c r="C59" s="108"/>
       <c r="D59" s="22"/>
       <c r="E59" s="83"/>
       <c r="F59" s="24"/>
@@ -4326,9 +4326,9 @@
       <c r="I59" s="26"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="100"/>
-      <c r="B60" s="103"/>
-      <c r="C60" s="97"/>
+      <c r="A60" s="105"/>
+      <c r="B60" s="107"/>
+      <c r="C60" s="109"/>
       <c r="D60" s="27"/>
       <c r="E60" s="28"/>
       <c r="F60" s="27"/>
@@ -4337,9 +4337,9 @@
       <c r="I60" s="28"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="100"/>
-      <c r="B61" s="103"/>
-      <c r="C61" s="97"/>
+      <c r="A61" s="105"/>
+      <c r="B61" s="107"/>
+      <c r="C61" s="109"/>
       <c r="D61" s="27"/>
       <c r="E61" s="28"/>
       <c r="F61" s="27"/>
@@ -4348,9 +4348,9 @@
       <c r="I61" s="28"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="100"/>
-      <c r="B62" s="103"/>
-      <c r="C62" s="97"/>
+      <c r="A62" s="105"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="109"/>
       <c r="D62" s="27"/>
       <c r="E62" s="28"/>
       <c r="F62" s="27"/>
@@ -4359,9 +4359,9 @@
       <c r="I62" s="28"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="100"/>
-      <c r="B63" s="103"/>
-      <c r="C63" s="98"/>
+      <c r="A63" s="105"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="110"/>
       <c r="D63" s="41"/>
       <c r="E63" s="33"/>
       <c r="F63" s="32"/>
@@ -4370,13 +4370,13 @@
       <c r="I63" s="33"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="99" t="s">
+      <c r="A64" s="104" t="s">
         <v>156</v>
       </c>
-      <c r="B64" s="102" t="s">
+      <c r="B64" s="106" t="s">
         <v>157</v>
       </c>
-      <c r="C64" s="96"/>
+      <c r="C64" s="108"/>
       <c r="D64" s="22"/>
       <c r="E64" s="83"/>
       <c r="F64" s="24"/>
@@ -4385,9 +4385,9 @@
       <c r="I64" s="26"/>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="100"/>
-      <c r="B65" s="103"/>
-      <c r="C65" s="97"/>
+      <c r="A65" s="105"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="109"/>
       <c r="D65" s="27"/>
       <c r="E65" s="28"/>
       <c r="F65" s="27"/>
@@ -4396,9 +4396,9 @@
       <c r="I65" s="28"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="100"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="97"/>
+      <c r="A66" s="105"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="109"/>
       <c r="D66" s="27"/>
       <c r="E66" s="28"/>
       <c r="F66" s="27"/>
@@ -4407,9 +4407,9 @@
       <c r="I66" s="28"/>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="100"/>
-      <c r="B67" s="103"/>
-      <c r="C67" s="97"/>
+      <c r="A67" s="105"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="109"/>
       <c r="D67" s="27"/>
       <c r="E67" s="28"/>
       <c r="F67" s="27"/>
@@ -4418,9 +4418,9 @@
       <c r="I67" s="28"/>
     </row>
     <row r="68" spans="1:9">
-      <c r="A68" s="100"/>
-      <c r="B68" s="103"/>
-      <c r="C68" s="98"/>
+      <c r="A68" s="105"/>
+      <c r="B68" s="107"/>
+      <c r="C68" s="110"/>
       <c r="D68" s="41"/>
       <c r="E68" s="33"/>
       <c r="F68" s="32"/>
@@ -4429,13 +4429,13 @@
       <c r="I68" s="33"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="99" t="s">
+      <c r="A69" s="104" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="102" t="s">
+      <c r="B69" s="106" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="96"/>
+      <c r="C69" s="108"/>
       <c r="D69" s="22"/>
       <c r="E69" s="83"/>
       <c r="F69" s="24"/>
@@ -4444,9 +4444,9 @@
       <c r="I69" s="26"/>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="100"/>
-      <c r="B70" s="103"/>
-      <c r="C70" s="97"/>
+      <c r="A70" s="105"/>
+      <c r="B70" s="107"/>
+      <c r="C70" s="109"/>
       <c r="D70" s="27"/>
       <c r="E70" s="28"/>
       <c r="F70" s="27"/>
@@ -4455,9 +4455,9 @@
       <c r="I70" s="28"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="100"/>
-      <c r="B71" s="103"/>
-      <c r="C71" s="97"/>
+      <c r="A71" s="105"/>
+      <c r="B71" s="107"/>
+      <c r="C71" s="109"/>
       <c r="D71" s="27"/>
       <c r="E71" s="28"/>
       <c r="F71" s="27"/>
@@ -4466,9 +4466,9 @@
       <c r="I71" s="28"/>
     </row>
     <row r="72" spans="1:9">
-      <c r="A72" s="100"/>
-      <c r="B72" s="103"/>
-      <c r="C72" s="97"/>
+      <c r="A72" s="105"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="109"/>
       <c r="D72" s="27"/>
       <c r="E72" s="28"/>
       <c r="F72" s="27"/>
@@ -4477,9 +4477,9 @@
       <c r="I72" s="28"/>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="100"/>
-      <c r="B73" s="103"/>
-      <c r="C73" s="98"/>
+      <c r="A73" s="105"/>
+      <c r="B73" s="107"/>
+      <c r="C73" s="110"/>
       <c r="D73" s="41"/>
       <c r="E73" s="33"/>
       <c r="F73" s="32"/>
@@ -4488,13 +4488,13 @@
       <c r="I73" s="33"/>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="99" t="s">
+      <c r="A74" s="104" t="s">
         <v>160</v>
       </c>
-      <c r="B74" s="102" t="s">
+      <c r="B74" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="C74" s="96"/>
+      <c r="C74" s="108"/>
       <c r="D74" s="22"/>
       <c r="E74" s="83"/>
       <c r="F74" s="24"/>
@@ -4503,9 +4503,9 @@
       <c r="I74" s="26"/>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="100"/>
-      <c r="B75" s="103"/>
-      <c r="C75" s="97"/>
+      <c r="A75" s="105"/>
+      <c r="B75" s="107"/>
+      <c r="C75" s="109"/>
       <c r="D75" s="27"/>
       <c r="E75" s="28"/>
       <c r="F75" s="27"/>
@@ -4514,9 +4514,9 @@
       <c r="I75" s="28"/>
     </row>
     <row r="76" spans="1:9">
-      <c r="A76" s="100"/>
-      <c r="B76" s="103"/>
-      <c r="C76" s="97"/>
+      <c r="A76" s="105"/>
+      <c r="B76" s="107"/>
+      <c r="C76" s="109"/>
       <c r="D76" s="27"/>
       <c r="E76" s="28"/>
       <c r="F76" s="27"/>
@@ -4525,9 +4525,9 @@
       <c r="I76" s="28"/>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="100"/>
-      <c r="B77" s="103"/>
-      <c r="C77" s="97"/>
+      <c r="A77" s="105"/>
+      <c r="B77" s="107"/>
+      <c r="C77" s="109"/>
       <c r="D77" s="27"/>
       <c r="E77" s="28"/>
       <c r="F77" s="27"/>
@@ -4536,9 +4536,9 @@
       <c r="I77" s="28"/>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="101"/>
-      <c r="B78" s="104"/>
-      <c r="C78" s="98"/>
+      <c r="A78" s="111"/>
+      <c r="B78" s="112"/>
+      <c r="C78" s="110"/>
       <c r="D78" s="41"/>
       <c r="E78" s="33"/>
       <c r="F78" s="32"/>
@@ -4547,13 +4547,13 @@
       <c r="I78" s="33"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="99" t="s">
+      <c r="A79" s="104" t="s">
         <v>163</v>
       </c>
-      <c r="B79" s="102" t="s">
+      <c r="B79" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="C79" s="96"/>
+      <c r="C79" s="108"/>
       <c r="D79" s="22"/>
       <c r="E79" s="83"/>
       <c r="F79" s="24"/>
@@ -4562,9 +4562,9 @@
       <c r="I79" s="26"/>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="100"/>
-      <c r="B80" s="103"/>
-      <c r="C80" s="97"/>
+      <c r="A80" s="105"/>
+      <c r="B80" s="107"/>
+      <c r="C80" s="109"/>
       <c r="D80" s="27"/>
       <c r="E80" s="28"/>
       <c r="F80" s="27"/>
@@ -4573,9 +4573,9 @@
       <c r="I80" s="28"/>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="100"/>
-      <c r="B81" s="103"/>
-      <c r="C81" s="97"/>
+      <c r="A81" s="105"/>
+      <c r="B81" s="107"/>
+      <c r="C81" s="109"/>
       <c r="D81" s="27"/>
       <c r="E81" s="28"/>
       <c r="F81" s="27"/>
@@ -4584,9 +4584,9 @@
       <c r="I81" s="28"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="100"/>
-      <c r="B82" s="103"/>
-      <c r="C82" s="97"/>
+      <c r="A82" s="105"/>
+      <c r="B82" s="107"/>
+      <c r="C82" s="109"/>
       <c r="D82" s="27"/>
       <c r="E82" s="28"/>
       <c r="F82" s="27"/>
@@ -4595,9 +4595,9 @@
       <c r="I82" s="28"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="101"/>
-      <c r="B83" s="104"/>
-      <c r="C83" s="98"/>
+      <c r="A83" s="111"/>
+      <c r="B83" s="112"/>
+      <c r="C83" s="110"/>
       <c r="D83" s="41"/>
       <c r="E83" s="33"/>
       <c r="F83" s="32"/>
@@ -4607,26 +4607,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="C34:C38"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="C39:C43"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
     <mergeCell ref="C44:C48"/>
     <mergeCell ref="C49:C53"/>
     <mergeCell ref="C54:C58"/>
@@ -4643,6 +4623,26 @@
     <mergeCell ref="B59:B63"/>
     <mergeCell ref="A64:A68"/>
     <mergeCell ref="B64:B68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="C34:C38"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="C39:C43"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>